<commit_message>
Fixed the 1st Testcase
</commit_message>
<xml_diff>
--- a/testdata/Book.xlsx
+++ b/testdata/Book.xlsx
@@ -14,7 +14,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A23:M24"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Courses</t>
   </si>
@@ -178,12 +178,16 @@
   </si>
   <si>
     <t>English (738)</t>
+  </si>
+  <si>
+    <t>Introduction to Front-End Development</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,9 +581,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.6328125" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.6328125"/>
+    <col min="2" max="2" customWidth="true" width="28.1796875"/>
+    <col min="3" max="3" customWidth="true" width="11.54296875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -599,24 +603,24 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>5</v>
       </c>
     </row>
@@ -635,9 +639,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="13.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.7265625"/>
+    <col min="2" max="2" customWidth="true" width="17.26953125"/>
+    <col min="3" max="3" customWidth="true" width="13.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -657,185 +661,185 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" t="s" s="0">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" t="s" s="0">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="B15" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" t="s" s="0">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+      <c r="B19" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" t="s" s="0">
         <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+      <c r="B21" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" t="s" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="B22" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="A24" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" t="s" s="0">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+      <c r="B25" t="s" s="0">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" t="s" s="0">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+      <c r="B26" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+      <c r="B27" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" t="s" s="0">
         <v>14</v>
       </c>
     </row>

</xml_diff>